<commit_message>
fixed many, many typos
</commit_message>
<xml_diff>
--- a/ClassComputerAssignments.xlsx
+++ b/ClassComputerAssignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ccrow/SynologyDrive/kubernetes-learning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB89AC4-0ACB-EB41-A3F9-C1180BD1A103}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DD2859-E21E-9C4C-80BA-844B1DD62EA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27400" yWindow="8100" windowWidth="25720" windowHeight="13480" xr2:uid="{BF274F19-62EC-1E4D-8F63-90CEC97917F4}"/>
+    <workbookView xWindow="25480" yWindow="8100" windowWidth="25720" windowHeight="13480" xr2:uid="{BF274F19-62EC-1E4D-8F63-90CEC97917F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Student</t>
   </si>
@@ -169,18 +169,6 @@
   </si>
   <si>
     <t>NickB</t>
-  </si>
-  <si>
-    <t>ccrowa01</t>
-  </si>
-  <si>
-    <t>ccrowa02</t>
-  </si>
-  <si>
-    <t>10.228.112.209</t>
-  </si>
-  <si>
-    <t>10.228.112.208</t>
   </si>
 </sst>
 </file>
@@ -548,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E9E472-C474-7142-B40C-ACF223797F1B}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -730,20 +718,6 @@
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>48</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>